<commit_message>
kinematics: add vz likelihood term, remove SHMR util, update STRRINGS
- llikelihood.py: expose xv_stream, add optional vz constraint using
  line-of-sight velocity when present in dict_data
- utils.py: remove halo_mass_from_stellar_mass (Moster+2013 SHMR)
- STRRINGS.xlsx: updated tracking spreadsheet

Co-Authored-By: Claude Sonnet 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/STRRINGS.xlsx
+++ b/STRRINGS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidchemaly/Documents/Cambridge/PhD_Projects/StreaMAX_fit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEDF0A43-CF98-B547-9156-E831A605A2F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9350BD34-9AF6-0945-BCAC-EC727E76CC40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="920" windowWidth="28800" windowHeight="16280" xr2:uid="{3DFC7EE5-590C-1B47-B680-0C0726C9184F}"/>
+    <workbookView xWindow="900" yWindow="660" windowWidth="19920" windowHeight="15980" xr2:uid="{3DFC7EE5-590C-1B47-B680-0C0726C9184F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="57">
   <si>
     <t>ESO079-003_GROUP_factor2.5_pixscale0.6</t>
   </si>
@@ -180,30 +180,9 @@
     <t>nan</t>
   </si>
   <si>
-    <t>bad?</t>
-  </si>
-  <si>
     <t>REJECT</t>
   </si>
   <si>
-    <t>calx207</t>
-  </si>
-  <si>
-    <t>calx208</t>
-  </si>
-  <si>
-    <t>cap002a</t>
-  </si>
-  <si>
-    <t>cap002b</t>
-  </si>
-  <si>
-    <t>cap002c</t>
-  </si>
-  <si>
-    <t>cap002d</t>
-  </si>
-  <si>
     <t>clip</t>
   </si>
   <si>
@@ -211,6 +190,24 @@
   </si>
   <si>
     <t>Name</t>
+  </si>
+  <si>
+    <t>gotta do it again with 2 extra data points</t>
+  </si>
+  <si>
+    <t>Do again on a bigger machine</t>
+  </si>
+  <si>
+    <t>to do</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>Elisabeth</t>
   </si>
 </sst>
 </file>
@@ -597,829 +594,944 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2CC44E2-1A8C-F545-86AE-10610759235C}">
-  <dimension ref="A1:K36"/>
+  <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="37" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" customWidth="1"/>
+    <col min="4" max="4" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="B1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" t="s">
         <v>35</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>38</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>37</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>36</v>
       </c>
-      <c r="F1" t="s">
-        <v>55</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C2">
+        <v>54</v>
+      </c>
+      <c r="C2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2">
         <v>18000</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>1000</v>
       </c>
-      <c r="E2">
-        <v>9</v>
-      </c>
-      <c r="G2" s="1" t="s">
+      <c r="F2">
+        <v>9</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="K2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C3">
+        <v>54</v>
+      </c>
+      <c r="C3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3">
         <v>24000</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>2000</v>
       </c>
-      <c r="E3">
-        <v>9</v>
-      </c>
-      <c r="G3" s="1" t="s">
+      <c r="F3">
+        <v>9</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C4">
+        <v>54</v>
+      </c>
+      <c r="C4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4">
         <v>25500</v>
       </c>
-      <c r="D4">
-        <v>1500</v>
-      </c>
       <c r="E4">
-        <v>9</v>
-      </c>
-      <c r="G4" s="1">
+        <v>1500</v>
+      </c>
+      <c r="F4">
+        <v>9</v>
+      </c>
+      <c r="H4" s="1">
         <v>5071.1000000000004</v>
       </c>
-      <c r="H4" s="1">
+      <c r="I4" s="1">
         <v>6.1</v>
       </c>
-      <c r="I4" s="1">
+      <c r="J4" s="1">
         <v>9.6999999999999993</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C5">
+        <v>54</v>
+      </c>
+      <c r="C5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5">
         <v>49500</v>
       </c>
-      <c r="D5">
-        <v>1500</v>
-      </c>
       <c r="E5">
-        <v>9</v>
-      </c>
-      <c r="G5" s="1">
+        <v>1500</v>
+      </c>
+      <c r="F5">
+        <v>9</v>
+      </c>
+      <c r="H5" s="1">
         <v>4590.5</v>
       </c>
-      <c r="H5" s="1">
+      <c r="I5" s="1">
         <v>111.2</v>
       </c>
-      <c r="I5" s="1">
+      <c r="J5" s="1">
         <v>1.7</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="K5" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6">
+        <v>55</v>
+      </c>
+      <c r="C6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6">
         <v>13500</v>
       </c>
-      <c r="D6">
-        <v>1500</v>
-      </c>
       <c r="E6">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+        <v>1500</v>
+      </c>
+      <c r="F6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
-      </c>
-      <c r="C7">
+        <v>54</v>
+      </c>
+      <c r="C7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7">
         <v>37500</v>
       </c>
-      <c r="D7">
-        <v>1500</v>
-      </c>
       <c r="E7">
-        <v>9</v>
-      </c>
-      <c r="G7" s="1">
+        <v>1500</v>
+      </c>
+      <c r="F7">
+        <v>9</v>
+      </c>
+      <c r="H7" s="1">
         <v>3547.4</v>
       </c>
-      <c r="H7" s="1">
+      <c r="I7" s="1">
         <v>26.9</v>
       </c>
-      <c r="I7" s="1">
+      <c r="J7" s="1">
         <v>6.5</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="K7" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>41</v>
-      </c>
-      <c r="C8">
+        <v>54</v>
+      </c>
+      <c r="C8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8">
         <v>57000</v>
       </c>
-      <c r="D8">
-        <v>1500</v>
-      </c>
       <c r="E8">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+        <v>1500</v>
+      </c>
+      <c r="F8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>49</v>
-      </c>
-      <c r="C9">
+        <v>55</v>
+      </c>
+      <c r="C9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9">
         <v>73500</v>
       </c>
-      <c r="D9">
-        <v>1500</v>
-      </c>
       <c r="E9">
+        <v>1500</v>
+      </c>
+      <c r="F9">
         <v>4</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>1</v>
       </c>
-      <c r="G9" s="1">
+      <c r="H9" s="1">
         <v>1326.4</v>
       </c>
-      <c r="H9" s="1">
+      <c r="I9" s="1">
         <v>22</v>
       </c>
-      <c r="I9" s="1">
+      <c r="J9" s="1">
         <v>5</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="K9" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>50</v>
-      </c>
-      <c r="C10">
+        <v>54</v>
+      </c>
+      <c r="C10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10">
         <v>112500</v>
       </c>
-      <c r="D10">
-        <v>1500</v>
-      </c>
       <c r="E10">
+        <v>1500</v>
+      </c>
+      <c r="F10">
         <v>4</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>1</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="H10" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
-      </c>
-      <c r="C11">
+        <v>54</v>
+      </c>
+      <c r="C11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11">
         <v>42000</v>
       </c>
-      <c r="D11">
-        <v>1500</v>
-      </c>
       <c r="E11">
-        <v>9</v>
-      </c>
-      <c r="G11" s="1">
+        <v>1500</v>
+      </c>
+      <c r="F11">
+        <v>9</v>
+      </c>
+      <c r="H11" s="1">
         <v>3870.6</v>
       </c>
-      <c r="H11" s="1">
+      <c r="I11" s="1">
         <v>16.7</v>
       </c>
-      <c r="I11" s="1">
+      <c r="J11" s="1">
         <v>4.7</v>
       </c>
-      <c r="J11" s="1" t="s">
+      <c r="K11" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>41</v>
-      </c>
-      <c r="C12">
+        <v>54</v>
+      </c>
+      <c r="C12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12">
         <v>12000</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>1000</v>
       </c>
-      <c r="E12">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F12">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>41</v>
-      </c>
-      <c r="C13">
+        <v>54</v>
+      </c>
+      <c r="C13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13">
         <v>10500</v>
       </c>
-      <c r="D13">
-        <v>1500</v>
-      </c>
       <c r="E13">
-        <v>9</v>
-      </c>
-      <c r="G13" s="1">
+        <v>1500</v>
+      </c>
+      <c r="F13">
+        <v>9</v>
+      </c>
+      <c r="H13" s="1">
         <v>1534.1</v>
       </c>
-      <c r="H13" s="1">
+      <c r="I13" s="1">
         <v>29.1</v>
       </c>
-      <c r="I13" s="1">
+      <c r="J13" s="1">
         <v>2.8</v>
       </c>
-      <c r="J13" s="1" t="s">
+      <c r="K13" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>41</v>
-      </c>
-      <c r="C14">
+        <v>54</v>
+      </c>
+      <c r="C14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14">
         <v>56000</v>
       </c>
-      <c r="D14">
+      <c r="E14">
         <v>2000</v>
       </c>
-      <c r="E14">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F14">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>41</v>
-      </c>
-      <c r="C15">
+        <v>55</v>
+      </c>
+      <c r="C15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15">
         <v>16500</v>
       </c>
-      <c r="D15">
-        <v>1500</v>
-      </c>
       <c r="E15">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+        <v>1500</v>
+      </c>
+      <c r="F15">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>41</v>
-      </c>
-      <c r="C16">
+        <v>54</v>
+      </c>
+      <c r="C16" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16">
         <v>21000</v>
       </c>
-      <c r="D16">
-        <v>1500</v>
-      </c>
       <c r="E16">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+        <v>1500</v>
+      </c>
+      <c r="F16">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>41</v>
-      </c>
-      <c r="C17">
+        <v>54</v>
+      </c>
+      <c r="C17" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17">
         <v>16500</v>
       </c>
-      <c r="D17">
-        <v>1500</v>
-      </c>
       <c r="E17">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+        <v>1500</v>
+      </c>
+      <c r="F17">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18">
+        <v>55</v>
+      </c>
+      <c r="C18" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18">
         <v>14000</v>
       </c>
-      <c r="D18">
+      <c r="E18">
         <v>1000</v>
       </c>
-      <c r="E18">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F18">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>41</v>
-      </c>
-      <c r="C19">
+        <v>54</v>
+      </c>
+      <c r="C19" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19">
         <v>42000</v>
       </c>
-      <c r="D19">
-        <v>1500</v>
-      </c>
       <c r="E19">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+        <v>1500</v>
+      </c>
+      <c r="F19">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>41</v>
-      </c>
-      <c r="C20">
+        <v>54</v>
+      </c>
+      <c r="C20" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20">
         <v>22500</v>
       </c>
-      <c r="D20">
-        <v>1500</v>
-      </c>
       <c r="E20">
-        <v>9</v>
-      </c>
-      <c r="K20" t="s">
+        <v>1500</v>
+      </c>
+      <c r="F20">
+        <v>9</v>
+      </c>
+      <c r="L20" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>41</v>
-      </c>
-      <c r="C21">
+        <v>55</v>
+      </c>
+      <c r="C21" t="s">
+        <v>41</v>
+      </c>
+      <c r="D21">
         <v>22500</v>
       </c>
-      <c r="D21">
-        <v>1500</v>
-      </c>
       <c r="E21">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+        <v>1500</v>
+      </c>
+      <c r="F21">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>41</v>
-      </c>
-      <c r="C22">
+        <v>54</v>
+      </c>
+      <c r="C22" t="s">
+        <v>41</v>
+      </c>
+      <c r="D22">
         <v>25500</v>
       </c>
-      <c r="D22">
-        <v>1500</v>
-      </c>
       <c r="E22">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+        <v>1500</v>
+      </c>
+      <c r="F22">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>21</v>
       </c>
       <c r="B23" t="s">
+        <v>54</v>
+      </c>
+      <c r="C23" t="s">
+        <v>53</v>
+      </c>
+      <c r="D23">
+        <v>75000</v>
+      </c>
+      <c r="E23">
+        <v>1500</v>
+      </c>
+      <c r="F23">
+        <v>4</v>
+      </c>
+      <c r="G23" s="2">
+        <v>1</v>
+      </c>
+      <c r="H23" s="1">
+        <v>5331.2</v>
+      </c>
+      <c r="I23" s="1">
+        <v>11.1</v>
+      </c>
+      <c r="J23" s="1">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L23" t="s">
         <v>51</v>
       </c>
-      <c r="C23">
-        <v>75000</v>
-      </c>
-      <c r="D23">
-        <v>1500</v>
-      </c>
-      <c r="E23">
-        <v>4</v>
-      </c>
-      <c r="F23" s="2">
-        <v>1</v>
-      </c>
-      <c r="G23" s="1">
-        <v>5331.2</v>
-      </c>
-      <c r="H23" s="1">
-        <v>11.1</v>
-      </c>
-      <c r="I23" s="1">
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>41</v>
-      </c>
-      <c r="C24">
+        <v>54</v>
+      </c>
+      <c r="C24" t="s">
+        <v>41</v>
+      </c>
+      <c r="D24">
         <v>12000</v>
       </c>
-      <c r="D24">
-        <v>1500</v>
-      </c>
       <c r="E24">
-        <v>9</v>
-      </c>
-      <c r="G24" s="1">
+        <v>1500</v>
+      </c>
+      <c r="F24">
+        <v>9</v>
+      </c>
+      <c r="H24" s="1">
         <v>5393.3</v>
       </c>
-      <c r="H24" s="1">
+      <c r="I24" s="1">
         <v>51</v>
       </c>
-      <c r="I24" s="1">
+      <c r="J24" s="1">
         <v>2.5</v>
       </c>
-      <c r="J24" s="1" t="s">
+      <c r="K24" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>41</v>
-      </c>
-      <c r="C25">
+        <v>54</v>
+      </c>
+      <c r="C25" t="s">
+        <v>41</v>
+      </c>
+      <c r="D25">
         <v>46500</v>
       </c>
-      <c r="D25">
-        <v>1500</v>
-      </c>
       <c r="E25">
-        <v>9</v>
-      </c>
-      <c r="K25" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+        <v>1500</v>
+      </c>
+      <c r="F25">
+        <v>9</v>
+      </c>
+      <c r="L25" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>52</v>
-      </c>
-      <c r="C26">
+        <v>54</v>
+      </c>
+      <c r="C26" t="s">
+        <v>41</v>
+      </c>
+      <c r="D26">
         <v>39000</v>
       </c>
-      <c r="D26">
-        <v>1500</v>
-      </c>
       <c r="E26">
+        <v>1500</v>
+      </c>
+      <c r="F26">
         <v>4</v>
       </c>
-      <c r="F26" s="2">
+      <c r="G26" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>41</v>
-      </c>
-      <c r="C27">
+        <v>54</v>
+      </c>
+      <c r="C27" t="s">
+        <v>41</v>
+      </c>
+      <c r="D27">
         <v>46000</v>
       </c>
-      <c r="D27">
+      <c r="E27">
         <v>1000</v>
       </c>
-      <c r="E27">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F27">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>26</v>
       </c>
       <c r="B28" t="s">
+        <v>54</v>
+      </c>
+      <c r="C28" t="s">
         <v>53</v>
       </c>
-      <c r="C28">
+      <c r="D28">
         <v>61500</v>
       </c>
-      <c r="D28">
-        <v>1500</v>
-      </c>
       <c r="E28">
+        <v>1500</v>
+      </c>
+      <c r="F28">
         <v>4</v>
       </c>
-      <c r="F28" s="2">
+      <c r="G28" s="2">
         <v>1</v>
       </c>
-      <c r="G28" s="1">
+      <c r="H28" s="1">
         <v>4862.5</v>
       </c>
-      <c r="H28" s="1">
+      <c r="I28" s="1">
         <v>11.3</v>
       </c>
-      <c r="I28" s="1">
+      <c r="J28" s="1">
         <v>5.5</v>
       </c>
-      <c r="J28" s="1" t="s">
+      <c r="K28" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>41</v>
-      </c>
-      <c r="C29">
+        <v>55</v>
+      </c>
+      <c r="C29" t="s">
+        <v>41</v>
+      </c>
+      <c r="D29">
         <v>24000</v>
       </c>
-      <c r="D29">
-        <v>1500</v>
-      </c>
       <c r="E29">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+        <v>1500</v>
+      </c>
+      <c r="F29">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>41</v>
-      </c>
-      <c r="C30">
+        <v>54</v>
+      </c>
+      <c r="C30" t="s">
+        <v>41</v>
+      </c>
+      <c r="D30">
         <v>16000</v>
       </c>
-      <c r="D30">
+      <c r="E30">
         <v>1000</v>
       </c>
-      <c r="E30">
-        <v>9</v>
-      </c>
-      <c r="K30" t="s">
+      <c r="F30">
+        <v>9</v>
+      </c>
+      <c r="L30" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>54</v>
-      </c>
-      <c r="C31">
+        <v>55</v>
+      </c>
+      <c r="C31" t="s">
+        <v>53</v>
+      </c>
+      <c r="D31">
         <v>61500</v>
       </c>
-      <c r="D31">
-        <v>1500</v>
-      </c>
       <c r="E31">
+        <v>1500</v>
+      </c>
+      <c r="F31">
         <v>4</v>
       </c>
-      <c r="F31" s="2">
+      <c r="G31" s="2">
         <v>1</v>
       </c>
-      <c r="G31" s="1">
+      <c r="H31" s="1">
         <v>1511</v>
       </c>
-      <c r="H31" s="1">
+      <c r="I31" s="1">
         <v>18.8</v>
       </c>
-      <c r="I31" s="1">
+      <c r="J31" s="1">
         <v>3.8</v>
       </c>
-      <c r="J31" s="1" t="s">
+      <c r="K31" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L31" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>41</v>
-      </c>
-      <c r="C32">
+        <v>54</v>
+      </c>
+      <c r="C32" t="s">
+        <v>41</v>
+      </c>
+      <c r="D32">
         <v>10000</v>
       </c>
-      <c r="D32">
+      <c r="E32">
         <v>1000</v>
       </c>
-      <c r="E32">
-        <v>9</v>
-      </c>
-      <c r="G32" s="1">
+      <c r="F32">
+        <v>9</v>
+      </c>
+      <c r="H32" s="1">
         <v>5191.8</v>
       </c>
-      <c r="H32" s="1">
+      <c r="I32" s="1">
         <v>33.5</v>
       </c>
-      <c r="I32" s="1">
+      <c r="J32" s="1">
         <v>8.9</v>
       </c>
-      <c r="J32" s="1" t="s">
+      <c r="K32" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>41</v>
-      </c>
-      <c r="C33">
+        <v>54</v>
+      </c>
+      <c r="C33" t="s">
+        <v>41</v>
+      </c>
+      <c r="D33">
         <v>52000</v>
       </c>
-      <c r="D33">
+      <c r="E33">
         <v>2000</v>
       </c>
-      <c r="E33">
+      <c r="F33">
         <v>4</v>
       </c>
-      <c r="G33" s="1">
+      <c r="H33" s="1">
         <v>5069.5</v>
       </c>
-      <c r="H33" s="1">
+      <c r="I33" s="1">
         <v>74.400000000000006</v>
       </c>
-      <c r="I33" s="1">
+      <c r="J33" s="1">
         <v>3.5</v>
       </c>
-      <c r="J33" s="1" t="s">
+      <c r="K33" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>41</v>
-      </c>
-      <c r="C34">
+        <v>55</v>
+      </c>
+      <c r="C34" t="s">
+        <v>41</v>
+      </c>
+      <c r="D34">
         <v>24000</v>
       </c>
-      <c r="D34">
+      <c r="E34">
         <v>1000</v>
       </c>
-      <c r="E34">
-        <v>9</v>
-      </c>
-      <c r="G34" t="s">
+      <c r="F34">
+        <v>9</v>
+      </c>
+      <c r="H34" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>41</v>
-      </c>
-      <c r="C35">
+        <v>54</v>
+      </c>
+      <c r="C35" t="s">
+        <v>41</v>
+      </c>
+      <c r="D35">
         <v>72000</v>
       </c>
-      <c r="D35">
-        <v>1500</v>
-      </c>
       <c r="E35">
+        <v>1500</v>
+      </c>
+      <c r="F35">
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>41</v>
-      </c>
-      <c r="C36">
+        <v>54</v>
+      </c>
+      <c r="C36" t="s">
+        <v>41</v>
+      </c>
+      <c r="D36">
         <v>33000</v>
       </c>
-      <c r="D36">
-        <v>1500</v>
-      </c>
       <c r="E36">
+        <v>1500</v>
+      </c>
+      <c r="F36">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
bring updated STRRINGS.xlsx from kinematics branch
Co-Authored-By: Claude Sonnet 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/STRRINGS.xlsx
+++ b/STRRINGS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidchemaly/Documents/Cambridge/PhD_Projects/StreaMAX_fit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEDF0A43-CF98-B547-9156-E831A605A2F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9350BD34-9AF6-0945-BCAC-EC727E76CC40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="920" windowWidth="28800" windowHeight="16280" xr2:uid="{3DFC7EE5-590C-1B47-B680-0C0726C9184F}"/>
+    <workbookView xWindow="900" yWindow="660" windowWidth="19920" windowHeight="15980" xr2:uid="{3DFC7EE5-590C-1B47-B680-0C0726C9184F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="57">
   <si>
     <t>ESO079-003_GROUP_factor2.5_pixscale0.6</t>
   </si>
@@ -180,30 +180,9 @@
     <t>nan</t>
   </si>
   <si>
-    <t>bad?</t>
-  </si>
-  <si>
     <t>REJECT</t>
   </si>
   <si>
-    <t>calx207</t>
-  </si>
-  <si>
-    <t>calx208</t>
-  </si>
-  <si>
-    <t>cap002a</t>
-  </si>
-  <si>
-    <t>cap002b</t>
-  </si>
-  <si>
-    <t>cap002c</t>
-  </si>
-  <si>
-    <t>cap002d</t>
-  </si>
-  <si>
     <t>clip</t>
   </si>
   <si>
@@ -211,6 +190,24 @@
   </si>
   <si>
     <t>Name</t>
+  </si>
+  <si>
+    <t>gotta do it again with 2 extra data points</t>
+  </si>
+  <si>
+    <t>Do again on a bigger machine</t>
+  </si>
+  <si>
+    <t>to do</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>Elisabeth</t>
   </si>
 </sst>
 </file>
@@ -597,829 +594,944 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2CC44E2-1A8C-F545-86AE-10610759235C}">
-  <dimension ref="A1:K36"/>
+  <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="37" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" customWidth="1"/>
+    <col min="4" max="4" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="B1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" t="s">
         <v>35</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>38</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>37</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>36</v>
       </c>
-      <c r="F1" t="s">
-        <v>55</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C2">
+        <v>54</v>
+      </c>
+      <c r="C2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2">
         <v>18000</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>1000</v>
       </c>
-      <c r="E2">
-        <v>9</v>
-      </c>
-      <c r="G2" s="1" t="s">
+      <c r="F2">
+        <v>9</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="K2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C3">
+        <v>54</v>
+      </c>
+      <c r="C3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3">
         <v>24000</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>2000</v>
       </c>
-      <c r="E3">
-        <v>9</v>
-      </c>
-      <c r="G3" s="1" t="s">
+      <c r="F3">
+        <v>9</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C4">
+        <v>54</v>
+      </c>
+      <c r="C4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4">
         <v>25500</v>
       </c>
-      <c r="D4">
-        <v>1500</v>
-      </c>
       <c r="E4">
-        <v>9</v>
-      </c>
-      <c r="G4" s="1">
+        <v>1500</v>
+      </c>
+      <c r="F4">
+        <v>9</v>
+      </c>
+      <c r="H4" s="1">
         <v>5071.1000000000004</v>
       </c>
-      <c r="H4" s="1">
+      <c r="I4" s="1">
         <v>6.1</v>
       </c>
-      <c r="I4" s="1">
+      <c r="J4" s="1">
         <v>9.6999999999999993</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C5">
+        <v>54</v>
+      </c>
+      <c r="C5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5">
         <v>49500</v>
       </c>
-      <c r="D5">
-        <v>1500</v>
-      </c>
       <c r="E5">
-        <v>9</v>
-      </c>
-      <c r="G5" s="1">
+        <v>1500</v>
+      </c>
+      <c r="F5">
+        <v>9</v>
+      </c>
+      <c r="H5" s="1">
         <v>4590.5</v>
       </c>
-      <c r="H5" s="1">
+      <c r="I5" s="1">
         <v>111.2</v>
       </c>
-      <c r="I5" s="1">
+      <c r="J5" s="1">
         <v>1.7</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="K5" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6">
+        <v>55</v>
+      </c>
+      <c r="C6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6">
         <v>13500</v>
       </c>
-      <c r="D6">
-        <v>1500</v>
-      </c>
       <c r="E6">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+        <v>1500</v>
+      </c>
+      <c r="F6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
-      </c>
-      <c r="C7">
+        <v>54</v>
+      </c>
+      <c r="C7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7">
         <v>37500</v>
       </c>
-      <c r="D7">
-        <v>1500</v>
-      </c>
       <c r="E7">
-        <v>9</v>
-      </c>
-      <c r="G7" s="1">
+        <v>1500</v>
+      </c>
+      <c r="F7">
+        <v>9</v>
+      </c>
+      <c r="H7" s="1">
         <v>3547.4</v>
       </c>
-      <c r="H7" s="1">
+      <c r="I7" s="1">
         <v>26.9</v>
       </c>
-      <c r="I7" s="1">
+      <c r="J7" s="1">
         <v>6.5</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="K7" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>41</v>
-      </c>
-      <c r="C8">
+        <v>54</v>
+      </c>
+      <c r="C8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8">
         <v>57000</v>
       </c>
-      <c r="D8">
-        <v>1500</v>
-      </c>
       <c r="E8">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+        <v>1500</v>
+      </c>
+      <c r="F8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>49</v>
-      </c>
-      <c r="C9">
+        <v>55</v>
+      </c>
+      <c r="C9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9">
         <v>73500</v>
       </c>
-      <c r="D9">
-        <v>1500</v>
-      </c>
       <c r="E9">
+        <v>1500</v>
+      </c>
+      <c r="F9">
         <v>4</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>1</v>
       </c>
-      <c r="G9" s="1">
+      <c r="H9" s="1">
         <v>1326.4</v>
       </c>
-      <c r="H9" s="1">
+      <c r="I9" s="1">
         <v>22</v>
       </c>
-      <c r="I9" s="1">
+      <c r="J9" s="1">
         <v>5</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="K9" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>50</v>
-      </c>
-      <c r="C10">
+        <v>54</v>
+      </c>
+      <c r="C10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10">
         <v>112500</v>
       </c>
-      <c r="D10">
-        <v>1500</v>
-      </c>
       <c r="E10">
+        <v>1500</v>
+      </c>
+      <c r="F10">
         <v>4</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>1</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="H10" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
-      </c>
-      <c r="C11">
+        <v>54</v>
+      </c>
+      <c r="C11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11">
         <v>42000</v>
       </c>
-      <c r="D11">
-        <v>1500</v>
-      </c>
       <c r="E11">
-        <v>9</v>
-      </c>
-      <c r="G11" s="1">
+        <v>1500</v>
+      </c>
+      <c r="F11">
+        <v>9</v>
+      </c>
+      <c r="H11" s="1">
         <v>3870.6</v>
       </c>
-      <c r="H11" s="1">
+      <c r="I11" s="1">
         <v>16.7</v>
       </c>
-      <c r="I11" s="1">
+      <c r="J11" s="1">
         <v>4.7</v>
       </c>
-      <c r="J11" s="1" t="s">
+      <c r="K11" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>41</v>
-      </c>
-      <c r="C12">
+        <v>54</v>
+      </c>
+      <c r="C12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12">
         <v>12000</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>1000</v>
       </c>
-      <c r="E12">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F12">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>41</v>
-      </c>
-      <c r="C13">
+        <v>54</v>
+      </c>
+      <c r="C13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13">
         <v>10500</v>
       </c>
-      <c r="D13">
-        <v>1500</v>
-      </c>
       <c r="E13">
-        <v>9</v>
-      </c>
-      <c r="G13" s="1">
+        <v>1500</v>
+      </c>
+      <c r="F13">
+        <v>9</v>
+      </c>
+      <c r="H13" s="1">
         <v>1534.1</v>
       </c>
-      <c r="H13" s="1">
+      <c r="I13" s="1">
         <v>29.1</v>
       </c>
-      <c r="I13" s="1">
+      <c r="J13" s="1">
         <v>2.8</v>
       </c>
-      <c r="J13" s="1" t="s">
+      <c r="K13" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>41</v>
-      </c>
-      <c r="C14">
+        <v>54</v>
+      </c>
+      <c r="C14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14">
         <v>56000</v>
       </c>
-      <c r="D14">
+      <c r="E14">
         <v>2000</v>
       </c>
-      <c r="E14">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F14">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>41</v>
-      </c>
-      <c r="C15">
+        <v>55</v>
+      </c>
+      <c r="C15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15">
         <v>16500</v>
       </c>
-      <c r="D15">
-        <v>1500</v>
-      </c>
       <c r="E15">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+        <v>1500</v>
+      </c>
+      <c r="F15">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>41</v>
-      </c>
-      <c r="C16">
+        <v>54</v>
+      </c>
+      <c r="C16" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16">
         <v>21000</v>
       </c>
-      <c r="D16">
-        <v>1500</v>
-      </c>
       <c r="E16">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+        <v>1500</v>
+      </c>
+      <c r="F16">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>41</v>
-      </c>
-      <c r="C17">
+        <v>54</v>
+      </c>
+      <c r="C17" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17">
         <v>16500</v>
       </c>
-      <c r="D17">
-        <v>1500</v>
-      </c>
       <c r="E17">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+        <v>1500</v>
+      </c>
+      <c r="F17">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18">
+        <v>55</v>
+      </c>
+      <c r="C18" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18">
         <v>14000</v>
       </c>
-      <c r="D18">
+      <c r="E18">
         <v>1000</v>
       </c>
-      <c r="E18">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F18">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>41</v>
-      </c>
-      <c r="C19">
+        <v>54</v>
+      </c>
+      <c r="C19" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19">
         <v>42000</v>
       </c>
-      <c r="D19">
-        <v>1500</v>
-      </c>
       <c r="E19">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+        <v>1500</v>
+      </c>
+      <c r="F19">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>41</v>
-      </c>
-      <c r="C20">
+        <v>54</v>
+      </c>
+      <c r="C20" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20">
         <v>22500</v>
       </c>
-      <c r="D20">
-        <v>1500</v>
-      </c>
       <c r="E20">
-        <v>9</v>
-      </c>
-      <c r="K20" t="s">
+        <v>1500</v>
+      </c>
+      <c r="F20">
+        <v>9</v>
+      </c>
+      <c r="L20" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>41</v>
-      </c>
-      <c r="C21">
+        <v>55</v>
+      </c>
+      <c r="C21" t="s">
+        <v>41</v>
+      </c>
+      <c r="D21">
         <v>22500</v>
       </c>
-      <c r="D21">
-        <v>1500</v>
-      </c>
       <c r="E21">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+        <v>1500</v>
+      </c>
+      <c r="F21">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>41</v>
-      </c>
-      <c r="C22">
+        <v>54</v>
+      </c>
+      <c r="C22" t="s">
+        <v>41</v>
+      </c>
+      <c r="D22">
         <v>25500</v>
       </c>
-      <c r="D22">
-        <v>1500</v>
-      </c>
       <c r="E22">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+        <v>1500</v>
+      </c>
+      <c r="F22">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>21</v>
       </c>
       <c r="B23" t="s">
+        <v>54</v>
+      </c>
+      <c r="C23" t="s">
+        <v>53</v>
+      </c>
+      <c r="D23">
+        <v>75000</v>
+      </c>
+      <c r="E23">
+        <v>1500</v>
+      </c>
+      <c r="F23">
+        <v>4</v>
+      </c>
+      <c r="G23" s="2">
+        <v>1</v>
+      </c>
+      <c r="H23" s="1">
+        <v>5331.2</v>
+      </c>
+      <c r="I23" s="1">
+        <v>11.1</v>
+      </c>
+      <c r="J23" s="1">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L23" t="s">
         <v>51</v>
       </c>
-      <c r="C23">
-        <v>75000</v>
-      </c>
-      <c r="D23">
-        <v>1500</v>
-      </c>
-      <c r="E23">
-        <v>4</v>
-      </c>
-      <c r="F23" s="2">
-        <v>1</v>
-      </c>
-      <c r="G23" s="1">
-        <v>5331.2</v>
-      </c>
-      <c r="H23" s="1">
-        <v>11.1</v>
-      </c>
-      <c r="I23" s="1">
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>41</v>
-      </c>
-      <c r="C24">
+        <v>54</v>
+      </c>
+      <c r="C24" t="s">
+        <v>41</v>
+      </c>
+      <c r="D24">
         <v>12000</v>
       </c>
-      <c r="D24">
-        <v>1500</v>
-      </c>
       <c r="E24">
-        <v>9</v>
-      </c>
-      <c r="G24" s="1">
+        <v>1500</v>
+      </c>
+      <c r="F24">
+        <v>9</v>
+      </c>
+      <c r="H24" s="1">
         <v>5393.3</v>
       </c>
-      <c r="H24" s="1">
+      <c r="I24" s="1">
         <v>51</v>
       </c>
-      <c r="I24" s="1">
+      <c r="J24" s="1">
         <v>2.5</v>
       </c>
-      <c r="J24" s="1" t="s">
+      <c r="K24" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>41</v>
-      </c>
-      <c r="C25">
+        <v>54</v>
+      </c>
+      <c r="C25" t="s">
+        <v>41</v>
+      </c>
+      <c r="D25">
         <v>46500</v>
       </c>
-      <c r="D25">
-        <v>1500</v>
-      </c>
       <c r="E25">
-        <v>9</v>
-      </c>
-      <c r="K25" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+        <v>1500</v>
+      </c>
+      <c r="F25">
+        <v>9</v>
+      </c>
+      <c r="L25" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>52</v>
-      </c>
-      <c r="C26">
+        <v>54</v>
+      </c>
+      <c r="C26" t="s">
+        <v>41</v>
+      </c>
+      <c r="D26">
         <v>39000</v>
       </c>
-      <c r="D26">
-        <v>1500</v>
-      </c>
       <c r="E26">
+        <v>1500</v>
+      </c>
+      <c r="F26">
         <v>4</v>
       </c>
-      <c r="F26" s="2">
+      <c r="G26" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>41</v>
-      </c>
-      <c r="C27">
+        <v>54</v>
+      </c>
+      <c r="C27" t="s">
+        <v>41</v>
+      </c>
+      <c r="D27">
         <v>46000</v>
       </c>
-      <c r="D27">
+      <c r="E27">
         <v>1000</v>
       </c>
-      <c r="E27">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F27">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>26</v>
       </c>
       <c r="B28" t="s">
+        <v>54</v>
+      </c>
+      <c r="C28" t="s">
         <v>53</v>
       </c>
-      <c r="C28">
+      <c r="D28">
         <v>61500</v>
       </c>
-      <c r="D28">
-        <v>1500</v>
-      </c>
       <c r="E28">
+        <v>1500</v>
+      </c>
+      <c r="F28">
         <v>4</v>
       </c>
-      <c r="F28" s="2">
+      <c r="G28" s="2">
         <v>1</v>
       </c>
-      <c r="G28" s="1">
+      <c r="H28" s="1">
         <v>4862.5</v>
       </c>
-      <c r="H28" s="1">
+      <c r="I28" s="1">
         <v>11.3</v>
       </c>
-      <c r="I28" s="1">
+      <c r="J28" s="1">
         <v>5.5</v>
       </c>
-      <c r="J28" s="1" t="s">
+      <c r="K28" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>41</v>
-      </c>
-      <c r="C29">
+        <v>55</v>
+      </c>
+      <c r="C29" t="s">
+        <v>41</v>
+      </c>
+      <c r="D29">
         <v>24000</v>
       </c>
-      <c r="D29">
-        <v>1500</v>
-      </c>
       <c r="E29">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+        <v>1500</v>
+      </c>
+      <c r="F29">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>41</v>
-      </c>
-      <c r="C30">
+        <v>54</v>
+      </c>
+      <c r="C30" t="s">
+        <v>41</v>
+      </c>
+      <c r="D30">
         <v>16000</v>
       </c>
-      <c r="D30">
+      <c r="E30">
         <v>1000</v>
       </c>
-      <c r="E30">
-        <v>9</v>
-      </c>
-      <c r="K30" t="s">
+      <c r="F30">
+        <v>9</v>
+      </c>
+      <c r="L30" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>54</v>
-      </c>
-      <c r="C31">
+        <v>55</v>
+      </c>
+      <c r="C31" t="s">
+        <v>53</v>
+      </c>
+      <c r="D31">
         <v>61500</v>
       </c>
-      <c r="D31">
-        <v>1500</v>
-      </c>
       <c r="E31">
+        <v>1500</v>
+      </c>
+      <c r="F31">
         <v>4</v>
       </c>
-      <c r="F31" s="2">
+      <c r="G31" s="2">
         <v>1</v>
       </c>
-      <c r="G31" s="1">
+      <c r="H31" s="1">
         <v>1511</v>
       </c>
-      <c r="H31" s="1">
+      <c r="I31" s="1">
         <v>18.8</v>
       </c>
-      <c r="I31" s="1">
+      <c r="J31" s="1">
         <v>3.8</v>
       </c>
-      <c r="J31" s="1" t="s">
+      <c r="K31" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L31" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>41</v>
-      </c>
-      <c r="C32">
+        <v>54</v>
+      </c>
+      <c r="C32" t="s">
+        <v>41</v>
+      </c>
+      <c r="D32">
         <v>10000</v>
       </c>
-      <c r="D32">
+      <c r="E32">
         <v>1000</v>
       </c>
-      <c r="E32">
-        <v>9</v>
-      </c>
-      <c r="G32" s="1">
+      <c r="F32">
+        <v>9</v>
+      </c>
+      <c r="H32" s="1">
         <v>5191.8</v>
       </c>
-      <c r="H32" s="1">
+      <c r="I32" s="1">
         <v>33.5</v>
       </c>
-      <c r="I32" s="1">
+      <c r="J32" s="1">
         <v>8.9</v>
       </c>
-      <c r="J32" s="1" t="s">
+      <c r="K32" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>41</v>
-      </c>
-      <c r="C33">
+        <v>54</v>
+      </c>
+      <c r="C33" t="s">
+        <v>41</v>
+      </c>
+      <c r="D33">
         <v>52000</v>
       </c>
-      <c r="D33">
+      <c r="E33">
         <v>2000</v>
       </c>
-      <c r="E33">
+      <c r="F33">
         <v>4</v>
       </c>
-      <c r="G33" s="1">
+      <c r="H33" s="1">
         <v>5069.5</v>
       </c>
-      <c r="H33" s="1">
+      <c r="I33" s="1">
         <v>74.400000000000006</v>
       </c>
-      <c r="I33" s="1">
+      <c r="J33" s="1">
         <v>3.5</v>
       </c>
-      <c r="J33" s="1" t="s">
+      <c r="K33" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>41</v>
-      </c>
-      <c r="C34">
+        <v>55</v>
+      </c>
+      <c r="C34" t="s">
+        <v>41</v>
+      </c>
+      <c r="D34">
         <v>24000</v>
       </c>
-      <c r="D34">
+      <c r="E34">
         <v>1000</v>
       </c>
-      <c r="E34">
-        <v>9</v>
-      </c>
-      <c r="G34" t="s">
+      <c r="F34">
+        <v>9</v>
+      </c>
+      <c r="H34" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>41</v>
-      </c>
-      <c r="C35">
+        <v>54</v>
+      </c>
+      <c r="C35" t="s">
+        <v>41</v>
+      </c>
+      <c r="D35">
         <v>72000</v>
       </c>
-      <c r="D35">
-        <v>1500</v>
-      </c>
       <c r="E35">
+        <v>1500</v>
+      </c>
+      <c r="F35">
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>41</v>
-      </c>
-      <c r="C36">
+        <v>54</v>
+      </c>
+      <c r="C36" t="s">
+        <v>41</v>
+      </c>
+      <c r="D36">
         <v>33000</v>
       </c>
-      <c r="D36">
-        <v>1500</v>
-      </c>
       <c r="E36">
+        <v>1500</v>
+      </c>
+      <c r="F36">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
var 4, points 1500
</commit_message>
<xml_diff>
--- a/STRRINGS.xlsx
+++ b/STRRINGS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidchemaly/Documents/Cambridge/PhD_Projects/StreaMAX_fit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9350BD34-9AF6-0945-BCAC-EC727E76CC40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25A81BB8-3E3C-1048-A785-C8348F2E35BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="900" yWindow="660" windowWidth="19920" windowHeight="15980" xr2:uid="{3DFC7EE5-590C-1B47-B680-0C0726C9184F}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="59">
   <si>
     <t>ESO079-003_GROUP_factor2.5_pixscale0.6</t>
   </si>
@@ -186,18 +185,9 @@
     <t>clip</t>
   </si>
   <si>
-    <t>try again?</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
-    <t>gotta do it again with 2 extra data points</t>
-  </si>
-  <si>
-    <t>Do again on a bigger machine</t>
-  </si>
-  <si>
     <t>to do</t>
   </si>
   <si>
@@ -208,6 +198,21 @@
   </si>
   <si>
     <t>Elisabeth</t>
+  </si>
+  <si>
+    <t>gotta change the track</t>
+  </si>
+  <si>
+    <t>Redo on bigger machine</t>
+  </si>
+  <si>
+    <t>redo with less points</t>
+  </si>
+  <si>
+    <t>give up? Ask Denis… or also change the track</t>
+  </si>
+  <si>
+    <t>redo with var 4 and 1500 points</t>
   </si>
 </sst>
 </file>
@@ -596,8 +601,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2CC44E2-1A8C-F545-86AE-10610759235C}">
   <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -610,10 +615,10 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C1" t="s">
         <v>35</v>
@@ -648,7 +653,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C2" t="s">
         <v>41</v>
@@ -664,9 +669,6 @@
       </c>
       <c r="H2" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="L2" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -674,7 +676,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C3" t="s">
         <v>41</v>
@@ -697,7 +699,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C4" t="s">
         <v>41</v>
@@ -729,7 +731,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C5" t="s">
         <v>41</v>
@@ -761,7 +763,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C6" t="s">
         <v>41</v>
@@ -781,7 +783,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C7" t="s">
         <v>41</v>
@@ -813,7 +815,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C8" t="s">
         <v>41</v>
@@ -833,10 +835,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C9" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D9">
         <v>73500</v>
@@ -861,6 +863,9 @@
       </c>
       <c r="K9" s="1" t="s">
         <v>44</v>
+      </c>
+      <c r="L9" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
@@ -868,10 +873,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C10" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D10">
         <v>112500</v>
@@ -888,13 +893,16 @@
       <c r="H10" s="1" t="s">
         <v>46</v>
       </c>
+      <c r="L10" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C11" t="s">
         <v>41</v>
@@ -926,7 +934,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C12" t="s">
         <v>41</v>
@@ -946,7 +954,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C13" t="s">
         <v>41</v>
@@ -978,7 +986,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C14" t="s">
         <v>41</v>
@@ -998,7 +1006,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C15" t="s">
         <v>41</v>
@@ -1018,7 +1026,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C16" t="s">
         <v>41</v>
@@ -1038,7 +1046,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C17" t="s">
         <v>41</v>
@@ -1058,7 +1066,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C18" t="s">
         <v>41</v>
@@ -1078,7 +1086,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C19" t="s">
         <v>41</v>
@@ -1098,7 +1106,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C20" t="s">
         <v>41</v>
@@ -1121,7 +1129,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C21" t="s">
         <v>41</v>
@@ -1141,7 +1149,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C22" t="s">
         <v>41</v>
@@ -1161,10 +1169,10 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C23" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D23">
         <v>75000</v>
@@ -1191,7 +1199,7 @@
         <v>44</v>
       </c>
       <c r="L23" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
@@ -1199,7 +1207,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C24" t="s">
         <v>41</v>
@@ -1231,7 +1239,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C25" t="s">
         <v>41</v>
@@ -1254,7 +1262,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C26" t="s">
         <v>41</v>
@@ -1277,7 +1285,7 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C27" t="s">
         <v>41</v>
@@ -1297,10 +1305,10 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C28" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D28">
         <v>61500</v>
@@ -1325,6 +1333,9 @@
       </c>
       <c r="K28" s="1" t="s">
         <v>44</v>
+      </c>
+      <c r="L28" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
@@ -1332,7 +1343,7 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C29" t="s">
         <v>41</v>
@@ -1352,7 +1363,7 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C30" t="s">
         <v>41</v>
@@ -1375,10 +1386,10 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C31" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D31">
         <v>61500</v>
@@ -1405,7 +1416,7 @@
         <v>44</v>
       </c>
       <c r="L31" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
@@ -1413,7 +1424,7 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C32" t="s">
         <v>41</v>
@@ -1445,7 +1456,7 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C33" t="s">
         <v>41</v>
@@ -1477,7 +1488,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C34" t="s">
         <v>41</v>
@@ -1500,7 +1511,7 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C35" t="s">
         <v>41</v>
@@ -1520,7 +1531,7 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C36" t="s">
         <v>41</v>

</xml_diff>

<commit_message>
saved new excel file
</commit_message>
<xml_diff>
--- a/STRRINGS.xlsx
+++ b/STRRINGS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidchemaly/Documents/Cambridge/PhD_Projects/StreaMAX_fit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25A81BB8-3E3C-1048-A785-C8348F2E35BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD7F5DB5-C7FB-3742-870D-EB24903C1413}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="900" yWindow="660" windowWidth="19920" windowHeight="15980" xr2:uid="{3DFC7EE5-590C-1B47-B680-0C0726C9184F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{3DFC7EE5-590C-1B47-B680-0C0726C9184F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="60">
   <si>
     <t>ESO079-003_GROUP_factor2.5_pixscale0.6</t>
   </si>
@@ -213,6 +213,9 @@
   </si>
   <si>
     <t>redo with var 4 and 1500 points</t>
+  </si>
+  <si>
+    <t>best</t>
   </si>
 </sst>
 </file>
@@ -601,8 +604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2CC44E2-1A8C-F545-86AE-10610759235C}">
   <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="N27" sqref="N27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -653,7 +656,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="C2" t="s">
         <v>41</v>
@@ -676,7 +679,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="C3" t="s">
         <v>41</v>
@@ -699,7 +702,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="C4" t="s">
         <v>41</v>
@@ -873,7 +876,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="C10" t="s">
         <v>50</v>
@@ -1026,7 +1029,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="C16" t="s">
         <v>41</v>
@@ -1169,7 +1172,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="C23" t="s">
         <v>50</v>
@@ -1262,7 +1265,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="C26" t="s">
         <v>41</v>
@@ -1285,7 +1288,7 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="C27" t="s">
         <v>41</v>
@@ -1531,7 +1534,7 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="C36" t="s">
         <v>41</v>

</xml_diff>

<commit_message>
mocking disk edge on
</commit_message>
<xml_diff>
--- a/STRRINGS.xlsx
+++ b/STRRINGS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidchemaly/Documents/Cambridge/PhD_Projects/StreaMAX_fit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD7F5DB5-C7FB-3742-870D-EB24903C1413}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D13C4BD0-7D79-D040-8CCC-F6325DDCAC8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{3DFC7EE5-590C-1B47-B680-0C0726C9184F}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" xr2:uid="{3DFC7EE5-590C-1B47-B680-0C0726C9184F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="61">
   <si>
     <t>ESO079-003_GROUP_factor2.5_pixscale0.6</t>
   </si>
@@ -216,6 +216,9 @@
   </si>
   <si>
     <t>best</t>
+  </si>
+  <si>
+    <t>sigma_ratio</t>
   </si>
 </sst>
 </file>
@@ -602,21 +605,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2CC44E2-1A8C-F545-86AE-10610759235C}">
-  <dimension ref="A1:L36"/>
+  <dimension ref="A1:M36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="37" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="4" max="4" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="11" customWidth="1"/>
+    <col min="5" max="5" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>49</v>
       </c>
@@ -624,928 +627,931 @@
         <v>53</v>
       </c>
       <c r="C1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" t="s">
         <v>35</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>38</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>37</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>36</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>48</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>59</v>
       </c>
-      <c r="C2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D2">
+      <c r="D2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2">
         <v>18000</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>1000</v>
       </c>
-      <c r="F2">
-        <v>9</v>
-      </c>
-      <c r="H2" s="1" t="s">
+      <c r="G2">
+        <v>9</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>59</v>
       </c>
-      <c r="C3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D3">
+      <c r="D3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3">
         <v>24000</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>2000</v>
       </c>
-      <c r="F3">
-        <v>9</v>
-      </c>
-      <c r="H3" s="1" t="s">
+      <c r="G3">
+        <v>9</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>59</v>
       </c>
-      <c r="C4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D4">
+      <c r="D4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4">
         <v>25500</v>
       </c>
-      <c r="E4">
-        <v>1500</v>
-      </c>
       <c r="F4">
-        <v>9</v>
-      </c>
-      <c r="H4" s="1">
+        <v>1500</v>
+      </c>
+      <c r="G4">
+        <v>9</v>
+      </c>
+      <c r="I4" s="1">
         <v>5071.1000000000004</v>
       </c>
-      <c r="I4" s="1">
+      <c r="J4" s="1">
         <v>6.1</v>
       </c>
-      <c r="J4" s="1">
+      <c r="K4" s="1">
         <v>9.6999999999999993</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="L4" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>51</v>
       </c>
-      <c r="C5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D5">
+      <c r="D5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5">
         <v>49500</v>
       </c>
-      <c r="E5">
-        <v>1500</v>
-      </c>
       <c r="F5">
-        <v>9</v>
-      </c>
-      <c r="H5" s="1">
+        <v>1500</v>
+      </c>
+      <c r="G5">
+        <v>9</v>
+      </c>
+      <c r="I5" s="1">
         <v>4590.5</v>
       </c>
-      <c r="I5" s="1">
+      <c r="J5" s="1">
         <v>111.2</v>
       </c>
-      <c r="J5" s="1">
+      <c r="K5" s="1">
         <v>1.7</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="L5" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>52</v>
       </c>
-      <c r="C6" t="s">
-        <v>41</v>
-      </c>
-      <c r="D6">
+      <c r="D6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6">
         <v>13500</v>
       </c>
-      <c r="E6">
-        <v>1500</v>
-      </c>
       <c r="F6">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+        <v>1500</v>
+      </c>
+      <c r="G6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>51</v>
       </c>
-      <c r="C7" t="s">
-        <v>41</v>
-      </c>
-      <c r="D7">
+      <c r="D7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7">
         <v>37500</v>
       </c>
-      <c r="E7">
-        <v>1500</v>
-      </c>
       <c r="F7">
-        <v>9</v>
-      </c>
-      <c r="H7" s="1">
+        <v>1500</v>
+      </c>
+      <c r="G7">
+        <v>9</v>
+      </c>
+      <c r="I7" s="1">
         <v>3547.4</v>
       </c>
-      <c r="I7" s="1">
+      <c r="J7" s="1">
         <v>26.9</v>
       </c>
-      <c r="J7" s="1">
+      <c r="K7" s="1">
         <v>6.5</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="L7" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8" t="s">
         <v>51</v>
       </c>
-      <c r="C8" t="s">
-        <v>41</v>
-      </c>
-      <c r="D8">
+      <c r="D8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8">
         <v>57000</v>
       </c>
-      <c r="E8">
-        <v>1500</v>
-      </c>
       <c r="F8">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+        <v>1500</v>
+      </c>
+      <c r="G8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9" t="s">
         <v>52</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>50</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>73500</v>
       </c>
-      <c r="E9">
-        <v>1500</v>
-      </c>
       <c r="F9">
+        <v>1500</v>
+      </c>
+      <c r="G9">
         <v>4</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>1</v>
       </c>
-      <c r="H9" s="1">
+      <c r="I9" s="1">
         <v>1326.4</v>
       </c>
-      <c r="I9" s="1">
+      <c r="J9" s="1">
         <v>22</v>
       </c>
-      <c r="J9" s="1">
+      <c r="K9" s="1">
         <v>5</v>
       </c>
-      <c r="K9" s="1" t="s">
+      <c r="L9" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="L9" t="s">
+      <c r="M9" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="B10" t="s">
         <v>59</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>50</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>112500</v>
       </c>
-      <c r="E10">
-        <v>1500</v>
-      </c>
       <c r="F10">
+        <v>1500</v>
+      </c>
+      <c r="G10">
         <v>4</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>1</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="I10" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="L10" t="s">
+      <c r="M10" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
       <c r="B11" t="s">
         <v>51</v>
       </c>
-      <c r="C11" t="s">
-        <v>41</v>
-      </c>
-      <c r="D11">
+      <c r="D11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11">
         <v>42000</v>
       </c>
-      <c r="E11">
-        <v>1500</v>
-      </c>
       <c r="F11">
-        <v>9</v>
-      </c>
-      <c r="H11" s="1">
+        <v>1500</v>
+      </c>
+      <c r="G11">
+        <v>9</v>
+      </c>
+      <c r="I11" s="1">
         <v>3870.6</v>
       </c>
-      <c r="I11" s="1">
+      <c r="J11" s="1">
         <v>16.7</v>
       </c>
-      <c r="J11" s="1">
+      <c r="K11" s="1">
         <v>4.7</v>
       </c>
-      <c r="K11" s="1" t="s">
+      <c r="L11" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
       <c r="B12" t="s">
         <v>51</v>
       </c>
-      <c r="C12" t="s">
-        <v>41</v>
-      </c>
-      <c r="D12">
+      <c r="D12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12">
         <v>12000</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>1000</v>
       </c>
-      <c r="F12">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="G12">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
       <c r="B13" t="s">
         <v>51</v>
       </c>
-      <c r="C13" t="s">
-        <v>41</v>
-      </c>
-      <c r="D13">
+      <c r="D13" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13">
         <v>10500</v>
       </c>
-      <c r="E13">
-        <v>1500</v>
-      </c>
       <c r="F13">
-        <v>9</v>
-      </c>
-      <c r="H13" s="1">
+        <v>1500</v>
+      </c>
+      <c r="G13">
+        <v>9</v>
+      </c>
+      <c r="I13" s="1">
         <v>1534.1</v>
       </c>
-      <c r="I13" s="1">
+      <c r="J13" s="1">
         <v>29.1</v>
       </c>
-      <c r="J13" s="1">
+      <c r="K13" s="1">
         <v>2.8</v>
       </c>
-      <c r="K13" s="1" t="s">
+      <c r="L13" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
       <c r="B14" t="s">
         <v>51</v>
       </c>
-      <c r="C14" t="s">
-        <v>41</v>
-      </c>
-      <c r="D14">
+      <c r="D14" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14">
         <v>56000</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <v>2000</v>
       </c>
-      <c r="F14">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="G14">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
       <c r="B15" t="s">
         <v>52</v>
       </c>
-      <c r="C15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D15">
+      <c r="D15" t="s">
+        <v>41</v>
+      </c>
+      <c r="E15">
         <v>16500</v>
       </c>
-      <c r="E15">
-        <v>1500</v>
-      </c>
       <c r="F15">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+        <v>1500</v>
+      </c>
+      <c r="G15">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>14</v>
       </c>
       <c r="B16" t="s">
         <v>59</v>
       </c>
-      <c r="C16" t="s">
-        <v>41</v>
-      </c>
-      <c r="D16">
+      <c r="D16" t="s">
+        <v>41</v>
+      </c>
+      <c r="E16">
         <v>21000</v>
       </c>
-      <c r="E16">
-        <v>1500</v>
-      </c>
       <c r="F16">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+        <v>1500</v>
+      </c>
+      <c r="G16">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>15</v>
       </c>
       <c r="B17" t="s">
         <v>51</v>
       </c>
-      <c r="C17" t="s">
-        <v>41</v>
-      </c>
-      <c r="D17">
+      <c r="D17" t="s">
+        <v>41</v>
+      </c>
+      <c r="E17">
         <v>16500</v>
       </c>
-      <c r="E17">
-        <v>1500</v>
-      </c>
       <c r="F17">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+        <v>1500</v>
+      </c>
+      <c r="G17">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>16</v>
       </c>
       <c r="B18" t="s">
         <v>52</v>
       </c>
-      <c r="C18" t="s">
-        <v>41</v>
-      </c>
-      <c r="D18">
+      <c r="D18" t="s">
+        <v>41</v>
+      </c>
+      <c r="E18">
         <v>14000</v>
       </c>
-      <c r="E18">
+      <c r="F18">
         <v>1000</v>
       </c>
-      <c r="F18">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="G18">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>17</v>
       </c>
       <c r="B19" t="s">
         <v>51</v>
       </c>
-      <c r="C19" t="s">
-        <v>41</v>
-      </c>
-      <c r="D19">
+      <c r="D19" t="s">
+        <v>41</v>
+      </c>
+      <c r="E19">
         <v>42000</v>
       </c>
-      <c r="E19">
-        <v>1500</v>
-      </c>
       <c r="F19">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+        <v>1500</v>
+      </c>
+      <c r="G19">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>18</v>
       </c>
       <c r="B20" t="s">
         <v>51</v>
       </c>
-      <c r="C20" t="s">
-        <v>41</v>
-      </c>
-      <c r="D20">
+      <c r="D20" t="s">
+        <v>41</v>
+      </c>
+      <c r="E20">
         <v>22500</v>
       </c>
-      <c r="E20">
-        <v>1500</v>
-      </c>
       <c r="F20">
-        <v>9</v>
-      </c>
-      <c r="L20" t="s">
+        <v>1500</v>
+      </c>
+      <c r="G20">
+        <v>9</v>
+      </c>
+      <c r="M20" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>19</v>
       </c>
       <c r="B21" t="s">
         <v>52</v>
       </c>
-      <c r="C21" t="s">
-        <v>41</v>
-      </c>
-      <c r="D21">
+      <c r="D21" t="s">
+        <v>41</v>
+      </c>
+      <c r="E21">
         <v>22500</v>
       </c>
-      <c r="E21">
-        <v>1500</v>
-      </c>
       <c r="F21">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+        <v>1500</v>
+      </c>
+      <c r="G21">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>20</v>
       </c>
       <c r="B22" t="s">
         <v>51</v>
       </c>
-      <c r="C22" t="s">
-        <v>41</v>
-      </c>
-      <c r="D22">
+      <c r="D22" t="s">
+        <v>41</v>
+      </c>
+      <c r="E22">
         <v>25500</v>
       </c>
-      <c r="E22">
-        <v>1500</v>
-      </c>
       <c r="F22">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+        <v>1500</v>
+      </c>
+      <c r="G22">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>21</v>
       </c>
       <c r="B23" t="s">
         <v>59</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>50</v>
       </c>
-      <c r="D23">
+      <c r="E23">
         <v>75000</v>
       </c>
-      <c r="E23">
-        <v>1500</v>
-      </c>
       <c r="F23">
+        <v>1500</v>
+      </c>
+      <c r="G23">
         <v>4</v>
       </c>
-      <c r="G23" s="2">
+      <c r="H23" s="2">
         <v>1</v>
       </c>
-      <c r="H23" s="1">
+      <c r="I23" s="1">
         <v>5331.2</v>
       </c>
-      <c r="I23" s="1">
+      <c r="J23" s="1">
         <v>11.1</v>
       </c>
-      <c r="J23" s="1">
+      <c r="K23" s="1">
         <v>8.8000000000000007</v>
       </c>
-      <c r="K23" s="1" t="s">
+      <c r="L23" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="L23" t="s">
+      <c r="M23" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>22</v>
       </c>
       <c r="B24" t="s">
         <v>51</v>
       </c>
-      <c r="C24" t="s">
-        <v>41</v>
-      </c>
-      <c r="D24">
+      <c r="D24" t="s">
+        <v>41</v>
+      </c>
+      <c r="E24">
         <v>12000</v>
       </c>
-      <c r="E24">
-        <v>1500</v>
-      </c>
       <c r="F24">
-        <v>9</v>
-      </c>
-      <c r="H24" s="1">
+        <v>1500</v>
+      </c>
+      <c r="G24">
+        <v>9</v>
+      </c>
+      <c r="I24" s="1">
         <v>5393.3</v>
       </c>
-      <c r="I24" s="1">
-        <v>51</v>
-      </c>
       <c r="J24" s="1">
+        <v>51</v>
+      </c>
+      <c r="K24" s="1">
         <v>2.5</v>
       </c>
-      <c r="K24" s="1" t="s">
+      <c r="L24" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>23</v>
       </c>
       <c r="B25" t="s">
         <v>51</v>
       </c>
-      <c r="C25" t="s">
-        <v>41</v>
-      </c>
-      <c r="D25">
+      <c r="D25" t="s">
+        <v>41</v>
+      </c>
+      <c r="E25">
         <v>46500</v>
       </c>
-      <c r="E25">
-        <v>1500</v>
-      </c>
       <c r="F25">
-        <v>9</v>
-      </c>
-      <c r="L25" t="s">
+        <v>1500</v>
+      </c>
+      <c r="G25">
+        <v>9</v>
+      </c>
+      <c r="M25" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>24</v>
       </c>
       <c r="B26" t="s">
         <v>59</v>
       </c>
-      <c r="C26" t="s">
-        <v>41</v>
-      </c>
-      <c r="D26">
+      <c r="D26" t="s">
+        <v>41</v>
+      </c>
+      <c r="E26">
         <v>39000</v>
       </c>
-      <c r="E26">
-        <v>1500</v>
-      </c>
       <c r="F26">
+        <v>1500</v>
+      </c>
+      <c r="G26">
         <v>4</v>
       </c>
-      <c r="G26" s="2">
+      <c r="H26" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>25</v>
       </c>
       <c r="B27" t="s">
         <v>59</v>
       </c>
-      <c r="C27" t="s">
-        <v>41</v>
-      </c>
-      <c r="D27">
+      <c r="D27" t="s">
+        <v>41</v>
+      </c>
+      <c r="E27">
         <v>46000</v>
       </c>
-      <c r="E27">
+      <c r="F27">
         <v>1000</v>
       </c>
-      <c r="F27">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="G27">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>26</v>
       </c>
       <c r="B28" t="s">
         <v>51</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>50</v>
       </c>
-      <c r="D28">
+      <c r="E28">
         <v>61500</v>
       </c>
-      <c r="E28">
-        <v>1500</v>
-      </c>
       <c r="F28">
+        <v>1500</v>
+      </c>
+      <c r="G28">
         <v>4</v>
       </c>
-      <c r="G28" s="2">
+      <c r="H28" s="2">
         <v>1</v>
       </c>
-      <c r="H28" s="1">
+      <c r="I28" s="1">
         <v>4862.5</v>
       </c>
-      <c r="I28" s="1">
+      <c r="J28" s="1">
         <v>11.3</v>
       </c>
-      <c r="J28" s="1">
+      <c r="K28" s="1">
         <v>5.5</v>
       </c>
-      <c r="K28" s="1" t="s">
+      <c r="L28" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="L28" t="s">
+      <c r="M28" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>27</v>
       </c>
       <c r="B29" t="s">
         <v>52</v>
       </c>
-      <c r="C29" t="s">
-        <v>41</v>
-      </c>
-      <c r="D29">
+      <c r="D29" t="s">
+        <v>41</v>
+      </c>
+      <c r="E29">
         <v>24000</v>
       </c>
-      <c r="E29">
-        <v>1500</v>
-      </c>
       <c r="F29">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+        <v>1500</v>
+      </c>
+      <c r="G29">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>28</v>
       </c>
       <c r="B30" t="s">
         <v>51</v>
       </c>
-      <c r="C30" t="s">
-        <v>41</v>
-      </c>
-      <c r="D30">
+      <c r="D30" t="s">
+        <v>41</v>
+      </c>
+      <c r="E30">
         <v>16000</v>
       </c>
-      <c r="E30">
+      <c r="F30">
         <v>1000</v>
       </c>
-      <c r="F30">
-        <v>9</v>
-      </c>
-      <c r="L30" t="s">
+      <c r="G30">
+        <v>9</v>
+      </c>
+      <c r="M30" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>29</v>
       </c>
       <c r="B31" t="s">
         <v>52</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
         <v>50</v>
       </c>
-      <c r="D31">
+      <c r="E31">
         <v>61500</v>
       </c>
-      <c r="E31">
-        <v>1500</v>
-      </c>
       <c r="F31">
+        <v>1500</v>
+      </c>
+      <c r="G31">
         <v>4</v>
       </c>
-      <c r="G31" s="2">
+      <c r="H31" s="2">
         <v>1</v>
       </c>
-      <c r="H31" s="1">
+      <c r="I31" s="1">
         <v>1511</v>
       </c>
-      <c r="I31" s="1">
+      <c r="J31" s="1">
         <v>18.8</v>
       </c>
-      <c r="J31" s="1">
+      <c r="K31" s="1">
         <v>3.8</v>
       </c>
-      <c r="K31" s="1" t="s">
+      <c r="L31" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="L31" t="s">
+      <c r="M31" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>30</v>
       </c>
       <c r="B32" t="s">
         <v>51</v>
       </c>
-      <c r="C32" t="s">
-        <v>41</v>
-      </c>
-      <c r="D32">
+      <c r="D32" t="s">
+        <v>41</v>
+      </c>
+      <c r="E32">
         <v>10000</v>
       </c>
-      <c r="E32">
+      <c r="F32">
         <v>1000</v>
       </c>
-      <c r="F32">
-        <v>9</v>
-      </c>
-      <c r="H32" s="1">
+      <c r="G32">
+        <v>9</v>
+      </c>
+      <c r="I32" s="1">
         <v>5191.8</v>
       </c>
-      <c r="I32" s="1">
+      <c r="J32" s="1">
         <v>33.5</v>
       </c>
-      <c r="J32" s="1">
+      <c r="K32" s="1">
         <v>8.9</v>
       </c>
-      <c r="K32" s="1" t="s">
+      <c r="L32" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>31</v>
       </c>
       <c r="B33" t="s">
         <v>51</v>
       </c>
-      <c r="C33" t="s">
-        <v>41</v>
-      </c>
-      <c r="D33">
+      <c r="D33" t="s">
+        <v>41</v>
+      </c>
+      <c r="E33">
         <v>52000</v>
       </c>
-      <c r="E33">
+      <c r="F33">
         <v>2000</v>
       </c>
-      <c r="F33">
+      <c r="G33">
         <v>4</v>
       </c>
-      <c r="H33" s="1">
+      <c r="I33" s="1">
         <v>5069.5</v>
       </c>
-      <c r="I33" s="1">
+      <c r="J33" s="1">
         <v>74.400000000000006</v>
       </c>
-      <c r="J33" s="1">
+      <c r="K33" s="1">
         <v>3.5</v>
       </c>
-      <c r="K33" s="1" t="s">
+      <c r="L33" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>32</v>
       </c>
       <c r="B34" t="s">
         <v>52</v>
       </c>
-      <c r="C34" t="s">
-        <v>41</v>
-      </c>
-      <c r="D34">
+      <c r="D34" t="s">
+        <v>41</v>
+      </c>
+      <c r="E34">
         <v>24000</v>
       </c>
-      <c r="E34">
+      <c r="F34">
         <v>1000</v>
       </c>
-      <c r="F34">
-        <v>9</v>
-      </c>
-      <c r="H34" t="s">
+      <c r="G34">
+        <v>9</v>
+      </c>
+      <c r="I34" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>33</v>
       </c>
       <c r="B35" t="s">
         <v>51</v>
       </c>
-      <c r="C35" t="s">
-        <v>41</v>
-      </c>
-      <c r="D35">
+      <c r="D35" t="s">
+        <v>41</v>
+      </c>
+      <c r="E35">
         <v>72000</v>
       </c>
-      <c r="E35">
-        <v>1500</v>
-      </c>
       <c r="F35">
+        <v>1500</v>
+      </c>
+      <c r="G35">
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>34</v>
       </c>
       <c r="B36" t="s">
         <v>59</v>
       </c>
-      <c r="C36" t="s">
-        <v>41</v>
-      </c>
-      <c r="D36">
+      <c r="D36" t="s">
+        <v>41</v>
+      </c>
+      <c r="E36">
         <v>33000</v>
       </c>
-      <c r="E36">
-        <v>1500</v>
-      </c>
       <c r="F36">
+        <v>1500</v>
+      </c>
+      <c r="G36">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added sigma_ratio to excel
</commit_message>
<xml_diff>
--- a/STRRINGS.xlsx
+++ b/STRRINGS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidchemaly/Documents/Cambridge/PhD_Projects/StreaMAX_fit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D13C4BD0-7D79-D040-8CCC-F6325DDCAC8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C91C638-EDB3-5F4A-B233-18ADCEF8D0F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" xr2:uid="{3DFC7EE5-590C-1B47-B680-0C0726C9184F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{3DFC7EE5-590C-1B47-B680-0C0726C9184F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="62">
   <si>
     <t>ESO079-003_GROUP_factor2.5_pixscale0.6</t>
   </si>
@@ -219,6 +219,9 @@
   </si>
   <si>
     <t>sigma_ratio</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -605,10 +608,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2CC44E2-1A8C-F545-86AE-10610759235C}">
-  <dimension ref="A1:M36"/>
+  <dimension ref="A1:Q36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -617,9 +620,11 @@
     <col min="2" max="3" width="11" customWidth="1"/>
     <col min="5" max="5" width="17.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="37" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>49</v>
       </c>
@@ -657,13 +662,16 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>59</v>
       </c>
+      <c r="C2">
+        <v>78.654844507959666</v>
+      </c>
       <c r="D2" t="s">
         <v>41</v>
       </c>
@@ -679,14 +687,20 @@
       <c r="I2" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="Q2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>59</v>
       </c>
+      <c r="C3">
+        <v>65.698367298851593</v>
+      </c>
       <c r="D3" t="s">
         <v>41</v>
       </c>
@@ -702,14 +716,20 @@
       <c r="I3" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="Q3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>59</v>
       </c>
+      <c r="C4">
+        <v>53.953585879898611</v>
+      </c>
       <c r="D4" t="s">
         <v>41</v>
       </c>
@@ -734,14 +754,20 @@
       <c r="L4" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="Q4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>51</v>
       </c>
+      <c r="C5">
+        <v>59.80726881378898</v>
+      </c>
       <c r="D5" t="s">
         <v>41</v>
       </c>
@@ -766,14 +792,20 @@
       <c r="L5" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="Q5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>52</v>
       </c>
+      <c r="C6">
+        <v>66.486284026074728</v>
+      </c>
       <c r="D6" t="s">
         <v>41</v>
       </c>
@@ -786,14 +818,20 @@
       <c r="G6">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="Q6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>51</v>
       </c>
+      <c r="C7">
+        <v>82.504263953251424</v>
+      </c>
       <c r="D7" t="s">
         <v>41</v>
       </c>
@@ -818,14 +856,20 @@
       <c r="L7" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="Q7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8" t="s">
         <v>51</v>
       </c>
+      <c r="C8">
+        <v>64.840124127438841</v>
+      </c>
       <c r="D8" t="s">
         <v>41</v>
       </c>
@@ -838,14 +882,20 @@
       <c r="G8">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="Q8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9" t="s">
         <v>52</v>
       </c>
+      <c r="C9" t="s">
+        <v>61</v>
+      </c>
       <c r="D9" t="s">
         <v>50</v>
       </c>
@@ -876,14 +926,20 @@
       <c r="M9" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="Q9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="B10" t="s">
         <v>59</v>
       </c>
+      <c r="C10" t="s">
+        <v>61</v>
+      </c>
       <c r="D10" t="s">
         <v>50</v>
       </c>
@@ -905,13 +961,19 @@
       <c r="M10" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="Q10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
       <c r="B11" t="s">
         <v>51</v>
+      </c>
+      <c r="C11">
+        <v>69.873372668561842</v>
       </c>
       <c r="D11" t="s">
         <v>41</v>
@@ -937,14 +999,20 @@
       <c r="L11" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="Q11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
       <c r="B12" t="s">
         <v>51</v>
       </c>
+      <c r="C12">
+        <v>36.268930152835487</v>
+      </c>
       <c r="D12" t="s">
         <v>41</v>
       </c>
@@ -957,14 +1025,20 @@
       <c r="G12">
         <v>9</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="Q12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
       <c r="B13" t="s">
         <v>51</v>
       </c>
+      <c r="C13">
+        <v>90.542280136417446</v>
+      </c>
       <c r="D13" t="s">
         <v>41</v>
       </c>
@@ -989,14 +1063,20 @@
       <c r="L13" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="Q13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
       <c r="B14" t="s">
         <v>51</v>
       </c>
+      <c r="C14">
+        <v>87.693954714566871</v>
+      </c>
       <c r="D14" t="s">
         <v>41</v>
       </c>
@@ -1009,14 +1089,20 @@
       <c r="G14">
         <v>9</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="Q14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
       <c r="B15" t="s">
         <v>52</v>
       </c>
+      <c r="C15">
+        <v>81.947799671078101</v>
+      </c>
       <c r="D15" t="s">
         <v>41</v>
       </c>
@@ -1029,14 +1115,20 @@
       <c r="G15">
         <v>9</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="Q15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>14</v>
       </c>
       <c r="B16" t="s">
         <v>59</v>
       </c>
+      <c r="C16">
+        <v>51.447760576429062</v>
+      </c>
       <c r="D16" t="s">
         <v>41</v>
       </c>
@@ -1049,14 +1141,20 @@
       <c r="G16">
         <v>9</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="Q16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>15</v>
       </c>
       <c r="B17" t="s">
         <v>51</v>
       </c>
+      <c r="C17">
+        <v>45.471096843211953</v>
+      </c>
       <c r="D17" t="s">
         <v>41</v>
       </c>
@@ -1069,14 +1167,20 @@
       <c r="G17">
         <v>9</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="Q17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>16</v>
       </c>
       <c r="B18" t="s">
         <v>52</v>
       </c>
+      <c r="C18">
+        <v>68.342485013728535</v>
+      </c>
       <c r="D18" t="s">
         <v>41</v>
       </c>
@@ -1089,14 +1193,20 @@
       <c r="G18">
         <v>9</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="Q18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>17</v>
       </c>
       <c r="B19" t="s">
         <v>51</v>
       </c>
+      <c r="C19">
+        <v>63.807178135337203</v>
+      </c>
       <c r="D19" t="s">
         <v>41</v>
       </c>
@@ -1109,14 +1219,20 @@
       <c r="G19">
         <v>9</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="Q19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>18</v>
       </c>
       <c r="B20" t="s">
         <v>51</v>
       </c>
+      <c r="C20">
+        <v>31.692075915159261</v>
+      </c>
       <c r="D20" t="s">
         <v>41</v>
       </c>
@@ -1132,14 +1248,20 @@
       <c r="M20" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="Q20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>19</v>
       </c>
       <c r="B21" t="s">
         <v>52</v>
       </c>
+      <c r="C21">
+        <v>89.123003413701312</v>
+      </c>
       <c r="D21" t="s">
         <v>41</v>
       </c>
@@ -1152,14 +1274,20 @@
       <c r="G21">
         <v>9</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="Q21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>20</v>
       </c>
       <c r="B22" t="s">
         <v>51</v>
       </c>
+      <c r="C22">
+        <v>80.271706068618229</v>
+      </c>
       <c r="D22" t="s">
         <v>41</v>
       </c>
@@ -1172,14 +1300,20 @@
       <c r="G22">
         <v>9</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="Q22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>21</v>
       </c>
       <c r="B23" t="s">
         <v>59</v>
       </c>
+      <c r="C23" t="s">
+        <v>61</v>
+      </c>
       <c r="D23" t="s">
         <v>50</v>
       </c>
@@ -1210,14 +1344,20 @@
       <c r="M23" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="Q23" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>22</v>
       </c>
       <c r="B24" t="s">
         <v>51</v>
       </c>
+      <c r="C24">
+        <v>89.745617229461871</v>
+      </c>
       <c r="D24" t="s">
         <v>41</v>
       </c>
@@ -1242,14 +1382,20 @@
       <c r="L24" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="Q24" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>23</v>
       </c>
       <c r="B25" t="s">
         <v>51</v>
       </c>
+      <c r="C25">
+        <v>82.611830801977987</v>
+      </c>
       <c r="D25" t="s">
         <v>41</v>
       </c>
@@ -1265,14 +1411,20 @@
       <c r="M25" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="Q25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>24</v>
       </c>
       <c r="B26" t="s">
         <v>59</v>
       </c>
+      <c r="C26">
+        <v>41.381685153983703</v>
+      </c>
       <c r="D26" t="s">
         <v>41</v>
       </c>
@@ -1288,14 +1440,20 @@
       <c r="H26" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="Q26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>25</v>
       </c>
       <c r="B27" t="s">
         <v>59</v>
       </c>
+      <c r="C27">
+        <v>76.395308522288346</v>
+      </c>
       <c r="D27" t="s">
         <v>41</v>
       </c>
@@ -1308,14 +1466,20 @@
       <c r="G27">
         <v>9</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="Q27" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>26</v>
       </c>
       <c r="B28" t="s">
         <v>51</v>
       </c>
+      <c r="C28" t="s">
+        <v>61</v>
+      </c>
       <c r="D28" t="s">
         <v>50</v>
       </c>
@@ -1346,14 +1510,20 @@
       <c r="M28" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="Q28" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>27</v>
       </c>
       <c r="B29" t="s">
         <v>52</v>
       </c>
+      <c r="C29">
+        <v>70.553748491929099</v>
+      </c>
       <c r="D29" t="s">
         <v>41</v>
       </c>
@@ -1366,14 +1536,20 @@
       <c r="G29">
         <v>9</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="Q29" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>28</v>
       </c>
       <c r="B30" t="s">
         <v>51</v>
       </c>
+      <c r="C30">
+        <v>71.860842600437707</v>
+      </c>
       <c r="D30" t="s">
         <v>41</v>
       </c>
@@ -1389,14 +1565,20 @@
       <c r="M30" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="Q30" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>29</v>
       </c>
       <c r="B31" t="s">
         <v>52</v>
       </c>
+      <c r="C31" t="s">
+        <v>61</v>
+      </c>
       <c r="D31" t="s">
         <v>50</v>
       </c>
@@ -1427,13 +1609,19 @@
       <c r="M31" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="Q31" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>30</v>
       </c>
       <c r="B32" t="s">
         <v>51</v>
+      </c>
+      <c r="C32">
+        <v>80.096582091956719</v>
       </c>
       <c r="D32" t="s">
         <v>41</v>
@@ -1467,6 +1655,9 @@
       <c r="B33" t="s">
         <v>51</v>
       </c>
+      <c r="C33">
+        <v>82.389461370168149</v>
+      </c>
       <c r="D33" t="s">
         <v>41</v>
       </c>
@@ -1499,6 +1690,9 @@
       <c r="B34" t="s">
         <v>52</v>
       </c>
+      <c r="C34">
+        <v>64.873489847899037</v>
+      </c>
       <c r="D34" t="s">
         <v>41</v>
       </c>
@@ -1522,6 +1716,9 @@
       <c r="B35" t="s">
         <v>51</v>
       </c>
+      <c r="C35">
+        <v>70.815824382423372</v>
+      </c>
       <c r="D35" t="s">
         <v>41</v>
       </c>
@@ -1541,6 +1738,9 @@
       </c>
       <c r="B36" t="s">
         <v>59</v>
+      </c>
+      <c r="C36">
+        <v>61.312945662889689</v>
       </c>
       <c r="D36" t="s">
         <v>41</v>

</xml_diff>

<commit_message>
made null into 999
</commit_message>
<xml_diff>
--- a/STRRINGS.xlsx
+++ b/STRRINGS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidchemaly/Documents/Cambridge/PhD_Projects/StreaMAX_fit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C91C638-EDB3-5F4A-B233-18ADCEF8D0F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8475CA08-47CD-7241-AED1-FEFFC6E51365}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{3DFC7EE5-590C-1B47-B680-0C0726C9184F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="61">
   <si>
     <t>ESO079-003_GROUP_factor2.5_pixscale0.6</t>
   </si>
@@ -219,9 +219,6 @@
   </si>
   <si>
     <t>sigma_ratio</t>
-  </si>
-  <si>
-    <t>-</t>
   </si>
 </sst>
 </file>
@@ -611,7 +608,7 @@
   <dimension ref="A1:Q36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -893,8 +890,8 @@
       <c r="B9" t="s">
         <v>52</v>
       </c>
-      <c r="C9" t="s">
-        <v>61</v>
+      <c r="C9">
+        <v>999</v>
       </c>
       <c r="D9" t="s">
         <v>50</v>
@@ -937,8 +934,8 @@
       <c r="B10" t="s">
         <v>59</v>
       </c>
-      <c r="C10" t="s">
-        <v>61</v>
+      <c r="C10">
+        <v>999</v>
       </c>
       <c r="D10" t="s">
         <v>50</v>
@@ -1311,8 +1308,8 @@
       <c r="B23" t="s">
         <v>59</v>
       </c>
-      <c r="C23" t="s">
-        <v>61</v>
+      <c r="C23">
+        <v>999</v>
       </c>
       <c r="D23" t="s">
         <v>50</v>
@@ -1477,8 +1474,8 @@
       <c r="B28" t="s">
         <v>51</v>
       </c>
-      <c r="C28" t="s">
-        <v>61</v>
+      <c r="C28">
+        <v>999</v>
       </c>
       <c r="D28" t="s">
         <v>50</v>
@@ -1576,8 +1573,8 @@
       <c r="B31" t="s">
         <v>52</v>
       </c>
-      <c r="C31" t="s">
-        <v>61</v>
+      <c r="C31">
+        <v>999</v>
       </c>
       <c r="D31" t="s">
         <v>50</v>

</xml_diff>

<commit_message>
ready for population fits
</commit_message>
<xml_diff>
--- a/STRRINGS.xlsx
+++ b/STRRINGS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10222"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidchemaly/Documents/Cambridge/PhD_Projects/StreaMAX_fit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8475CA08-47CD-7241-AED1-FEFFC6E51365}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F009684-E6DE-4543-98EA-FEC803FF8AFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{3DFC7EE5-590C-1B47-B680-0C0726C9184F}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" xr2:uid="{3DFC7EE5-590C-1B47-B680-0C0726C9184F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="60">
   <si>
     <t>ESO079-003_GROUP_factor2.5_pixscale0.6</t>
   </si>
@@ -180,9 +180,6 @@
   </si>
   <si>
     <t>REJECT</t>
-  </si>
-  <si>
-    <t>clip</t>
   </si>
   <si>
     <t>Name</t>
@@ -225,7 +222,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -238,13 +235,6 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -267,10 +257,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -605,10 +594,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2CC44E2-1A8C-F545-86AE-10610759235C}">
-  <dimension ref="A1:Q36"/>
+  <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -616,20 +605,19 @@
     <col min="1" max="1" width="37" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="11" customWidth="1"/>
     <col min="5" max="5" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="37" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="37" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D1" t="s">
         <v>35</v>
@@ -643,28 +631,25 @@
       <c r="G1" t="s">
         <v>36</v>
       </c>
-      <c r="H1" t="s">
-        <v>48</v>
+      <c r="H1" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="L1" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C2">
         <v>78.654844507959666</v>
@@ -681,19 +666,16 @@
       <c r="G2">
         <v>9</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="Q2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C3">
         <v>65.698367298851593</v>
@@ -710,19 +692,16 @@
       <c r="G3">
         <v>9</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="Q3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C4">
         <v>53.953585879898611</v>
@@ -739,28 +718,25 @@
       <c r="G4">
         <v>9</v>
       </c>
+      <c r="H4" s="1">
+        <v>5071.1000000000004</v>
+      </c>
       <c r="I4" s="1">
-        <v>5071.1000000000004</v>
+        <v>6.1</v>
       </c>
       <c r="J4" s="1">
-        <v>6.1</v>
-      </c>
-      <c r="K4" s="1">
         <v>9.6999999999999993</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="Q4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C5">
         <v>59.80726881378898</v>
@@ -777,28 +753,25 @@
       <c r="G5">
         <v>9</v>
       </c>
+      <c r="H5" s="1">
+        <v>4590.5</v>
+      </c>
       <c r="I5" s="1">
-        <v>4590.5</v>
+        <v>111.2</v>
       </c>
       <c r="J5" s="1">
-        <v>111.2</v>
-      </c>
-      <c r="K5" s="1">
         <v>1.7</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="K5" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="Q5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C6">
         <v>66.486284026074728</v>
@@ -815,16 +788,13 @@
       <c r="G6">
         <v>9</v>
       </c>
-      <c r="Q6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C7">
         <v>82.504263953251424</v>
@@ -841,28 +811,25 @@
       <c r="G7">
         <v>9</v>
       </c>
+      <c r="H7" s="1">
+        <v>3547.4</v>
+      </c>
       <c r="I7" s="1">
-        <v>3547.4</v>
+        <v>26.9</v>
       </c>
       <c r="J7" s="1">
-        <v>26.9</v>
-      </c>
-      <c r="K7" s="1">
         <v>6.5</v>
       </c>
-      <c r="L7" s="1" t="s">
+      <c r="K7" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="Q7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C8">
         <v>64.840124127438841</v>
@@ -879,22 +846,19 @@
       <c r="G8">
         <v>9</v>
       </c>
-      <c r="Q8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C9">
         <v>999</v>
       </c>
       <c r="D9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E9">
         <v>73500</v>
@@ -905,40 +869,34 @@
       <c r="G9">
         <v>4</v>
       </c>
-      <c r="H9">
-        <v>1</v>
+      <c r="H9" s="1">
+        <v>1326.4</v>
       </c>
       <c r="I9" s="1">
-        <v>1326.4</v>
+        <v>22</v>
       </c>
       <c r="J9" s="1">
-        <v>22</v>
-      </c>
-      <c r="K9" s="1">
         <v>5</v>
       </c>
-      <c r="L9" s="1" t="s">
+      <c r="K9" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="M9" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="L9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C10">
         <v>999</v>
       </c>
       <c r="D10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E10">
         <v>112500</v>
@@ -949,25 +907,19 @@
       <c r="G10">
         <v>4</v>
       </c>
-      <c r="H10">
-        <v>1</v>
-      </c>
-      <c r="I10" s="1" t="s">
+      <c r="H10" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="M10" t="s">
-        <v>57</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="L10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C11">
         <v>69.873372668561842</v>
@@ -984,28 +936,25 @@
       <c r="G11">
         <v>9</v>
       </c>
+      <c r="H11" s="1">
+        <v>3870.6</v>
+      </c>
       <c r="I11" s="1">
-        <v>3870.6</v>
+        <v>16.7</v>
       </c>
       <c r="J11" s="1">
-        <v>16.7</v>
-      </c>
-      <c r="K11" s="1">
         <v>4.7</v>
       </c>
-      <c r="L11" s="1" t="s">
+      <c r="K11" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="Q11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C12">
         <v>36.268930152835487</v>
@@ -1022,16 +971,13 @@
       <c r="G12">
         <v>9</v>
       </c>
-      <c r="Q12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C13">
         <v>90.542280136417446</v>
@@ -1048,28 +994,25 @@
       <c r="G13">
         <v>9</v>
       </c>
+      <c r="H13" s="1">
+        <v>1534.1</v>
+      </c>
       <c r="I13" s="1">
-        <v>1534.1</v>
+        <v>29.1</v>
       </c>
       <c r="J13" s="1">
-        <v>29.1</v>
-      </c>
-      <c r="K13" s="1">
         <v>2.8</v>
       </c>
-      <c r="L13" s="1" t="s">
+      <c r="K13" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="Q13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C14">
         <v>87.693954714566871</v>
@@ -1086,16 +1029,13 @@
       <c r="G14">
         <v>9</v>
       </c>
-      <c r="Q14" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C15">
         <v>81.947799671078101</v>
@@ -1112,16 +1052,13 @@
       <c r="G15">
         <v>9</v>
       </c>
-      <c r="Q15" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C16">
         <v>51.447760576429062</v>
@@ -1138,16 +1075,13 @@
       <c r="G16">
         <v>9</v>
       </c>
-      <c r="Q16" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C17">
         <v>45.471096843211953</v>
@@ -1164,16 +1098,13 @@
       <c r="G17">
         <v>9</v>
       </c>
-      <c r="Q17" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C18">
         <v>68.342485013728535</v>
@@ -1190,16 +1121,13 @@
       <c r="G18">
         <v>9</v>
       </c>
-      <c r="Q18" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C19">
         <v>63.807178135337203</v>
@@ -1216,16 +1144,13 @@
       <c r="G19">
         <v>9</v>
       </c>
-      <c r="Q19" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C20">
         <v>31.692075915159261</v>
@@ -1242,19 +1167,16 @@
       <c r="G20">
         <v>9</v>
       </c>
-      <c r="M20" t="s">
+      <c r="L20" t="s">
         <v>47</v>
       </c>
-      <c r="Q20" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C21">
         <v>89.123003413701312</v>
@@ -1271,16 +1193,13 @@
       <c r="G21">
         <v>9</v>
       </c>
-      <c r="Q21" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C22">
         <v>80.271706068618229</v>
@@ -1297,60 +1216,51 @@
       <c r="G22">
         <v>9</v>
       </c>
-      <c r="Q22" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C23">
-        <v>999</v>
+        <v>65.171187042439499</v>
       </c>
       <c r="D23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E23">
-        <v>75000</v>
+        <v>48000</v>
       </c>
       <c r="F23">
         <v>1500</v>
       </c>
       <c r="G23">
-        <v>4</v>
-      </c>
-      <c r="H23" s="2">
-        <v>1</v>
+        <v>9</v>
+      </c>
+      <c r="H23" s="1">
+        <v>5331.2</v>
       </c>
       <c r="I23" s="1">
-        <v>5331.2</v>
+        <v>11.1</v>
       </c>
       <c r="J23" s="1">
-        <v>11.1</v>
-      </c>
-      <c r="K23" s="1">
         <v>8.8000000000000007</v>
       </c>
-      <c r="L23" s="1" t="s">
+      <c r="K23" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="M23" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q23" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="L23" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C24">
         <v>89.745617229461871</v>
@@ -1367,31 +1277,28 @@
       <c r="G24">
         <v>9</v>
       </c>
+      <c r="H24" s="1">
+        <v>5393.3</v>
+      </c>
       <c r="I24" s="1">
-        <v>5393.3</v>
+        <v>51</v>
       </c>
       <c r="J24" s="1">
-        <v>51</v>
-      </c>
-      <c r="K24" s="1">
         <v>2.5</v>
       </c>
-      <c r="L24" s="1" t="s">
+      <c r="K24" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="Q24" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C25">
-        <v>82.611830801977987</v>
+        <v>999</v>
       </c>
       <c r="D25" t="s">
         <v>41</v>
@@ -1405,19 +1312,16 @@
       <c r="G25">
         <v>9</v>
       </c>
-      <c r="M25" t="s">
+      <c r="L25" t="s">
         <v>47</v>
       </c>
-      <c r="Q25" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C26">
         <v>41.381685153983703</v>
@@ -1434,19 +1338,13 @@
       <c r="G26">
         <v>4</v>
       </c>
-      <c r="H26" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q26" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C27">
         <v>76.395308522288346</v>
@@ -1463,22 +1361,19 @@
       <c r="G27">
         <v>9</v>
       </c>
-      <c r="Q27" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C28">
-        <v>999</v>
+        <v>55.4591005444492</v>
       </c>
       <c r="D28" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E28">
         <v>61500</v>
@@ -1489,34 +1384,28 @@
       <c r="G28">
         <v>4</v>
       </c>
-      <c r="H28" s="2">
-        <v>1</v>
+      <c r="H28" s="1">
+        <v>4862.5</v>
       </c>
       <c r="I28" s="1">
-        <v>4862.5</v>
+        <v>11.3</v>
       </c>
       <c r="J28" s="1">
-        <v>11.3</v>
-      </c>
-      <c r="K28" s="1">
         <v>5.5</v>
       </c>
-      <c r="L28" s="1" t="s">
+      <c r="K28" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="M28" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q28" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="L28" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C29">
         <v>70.553748491929099</v>
@@ -1533,16 +1422,13 @@
       <c r="G29">
         <v>9</v>
       </c>
-      <c r="Q29" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C30">
         <v>71.860842600437707</v>
@@ -1559,25 +1445,22 @@
       <c r="G30">
         <v>9</v>
       </c>
-      <c r="M30" t="s">
+      <c r="L30" t="s">
         <v>47</v>
       </c>
-      <c r="Q30" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C31">
-        <v>999</v>
+        <v>99.333229096921201</v>
       </c>
       <c r="D31" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E31">
         <v>61500</v>
@@ -1588,34 +1471,28 @@
       <c r="G31">
         <v>4</v>
       </c>
-      <c r="H31" s="2">
-        <v>1</v>
+      <c r="H31" s="1">
+        <v>1511</v>
       </c>
       <c r="I31" s="1">
-        <v>1511</v>
+        <v>18.8</v>
       </c>
       <c r="J31" s="1">
-        <v>18.8</v>
-      </c>
-      <c r="K31" s="1">
         <v>3.8</v>
       </c>
-      <c r="L31" s="1" t="s">
+      <c r="K31" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="M31" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q31" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="L31" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C32">
         <v>80.096582091956719</v>
@@ -1632,25 +1509,25 @@
       <c r="G32">
         <v>9</v>
       </c>
+      <c r="H32" s="1">
+        <v>5191.8</v>
+      </c>
       <c r="I32" s="1">
-        <v>5191.8</v>
+        <v>33.5</v>
       </c>
       <c r="J32" s="1">
-        <v>33.5</v>
-      </c>
-      <c r="K32" s="1">
         <v>8.9</v>
       </c>
-      <c r="L32" s="1" t="s">
+      <c r="K32" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C33">
         <v>82.389461370168149</v>
@@ -1667,25 +1544,25 @@
       <c r="G33">
         <v>4</v>
       </c>
+      <c r="H33" s="1">
+        <v>5069.5</v>
+      </c>
       <c r="I33" s="1">
-        <v>5069.5</v>
+        <v>74.400000000000006</v>
       </c>
       <c r="J33" s="1">
-        <v>74.400000000000006</v>
-      </c>
-      <c r="K33" s="1">
         <v>3.5</v>
       </c>
-      <c r="L33" s="1" t="s">
+      <c r="K33" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C34">
         <v>64.873489847899037</v>
@@ -1702,16 +1579,16 @@
       <c r="G34">
         <v>9</v>
       </c>
-      <c r="I34" t="s">
+      <c r="H34" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C35">
         <v>70.815824382423372</v>
@@ -1729,12 +1606,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C36">
         <v>61.312945662889689</v>

</xml_diff>